<commit_message>
creating json now from excel with python
</commit_message>
<xml_diff>
--- a/Odds.xlsx
+++ b/Odds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aqua\Documents\GitHub\PoeProfit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC3F635-E6DC-492B-9E92-6F92D4EF8D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74AD991B-C1D9-4CB0-B96C-34D13C5B463D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="31560" windowHeight="15435" xr2:uid="{577F8554-80CD-4CC0-9DB5-09CB9B2401F0}"/>
+    <workbookView xWindow="1575" yWindow="3420" windowWidth="31560" windowHeight="15435" xr2:uid="{577F8554-80CD-4CC0-9DB5-09CB9B2401F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
   <si>
     <t>shaper</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Talented</t>
   </si>
   <si>
-    <t>Uber</t>
-  </si>
-  <si>
     <t>Fragment of Knowledge</t>
   </si>
   <si>
@@ -71,12 +68,6 @@
     <t>Starforge</t>
   </si>
   <si>
-    <t>Solsice Vigil</t>
-  </si>
-  <si>
-    <t>Echoes of Cremation</t>
-  </si>
-  <si>
     <t>Sublime Vision</t>
   </si>
   <si>
@@ -84,6 +75,255 @@
   </si>
   <si>
     <t>Orb of Dominance</t>
+  </si>
+  <si>
+    <t>boss</t>
+  </si>
+  <si>
+    <t>elder</t>
+  </si>
+  <si>
+    <t>Fragment of Terror</t>
+  </si>
+  <si>
+    <t>Fragment of Emptiness</t>
+  </si>
+  <si>
+    <t>Cyclopean Coil</t>
+  </si>
+  <si>
+    <t>Nebuloch</t>
+  </si>
+  <si>
+    <t>Hopeshredder</t>
+  </si>
+  <si>
+    <t>Shimmeron</t>
+  </si>
+  <si>
+    <t>Any Impresence</t>
+  </si>
+  <si>
+    <t>Watchers Eye</t>
+  </si>
+  <si>
+    <t>85 Area</t>
+  </si>
+  <si>
+    <t>eater</t>
+  </si>
+  <si>
+    <t>The Gluttonous Tide</t>
+  </si>
+  <si>
+    <t>Inextricable Fate</t>
+  </si>
+  <si>
+    <t>Ashes of the Stars</t>
+  </si>
+  <si>
+    <t>Melding of the Flesh</t>
+  </si>
+  <si>
+    <t>Forbidden Flesh</t>
+  </si>
+  <si>
+    <t>Visceral Reliquary Key</t>
+  </si>
+  <si>
+    <t>Exceptional Eldritch Ichor</t>
+  </si>
+  <si>
+    <t>exarch</t>
+  </si>
+  <si>
+    <t>The Annihilating Light</t>
+  </si>
+  <si>
+    <t>Dawnbreaker</t>
+  </si>
+  <si>
+    <t>Dissolution of the Flesh</t>
+  </si>
+  <si>
+    <t>Crystallised Omniscience</t>
+  </si>
+  <si>
+    <t>Forbidden Flame</t>
+  </si>
+  <si>
+    <t>Archive Reliquary Key</t>
+  </si>
+  <si>
+    <t>Exceptional Eldritch Ember</t>
+  </si>
+  <si>
+    <t>atziri</t>
+  </si>
+  <si>
+    <t>Atziris Promise</t>
+  </si>
+  <si>
+    <t>Atziris Step</t>
+  </si>
+  <si>
+    <t>Doryanis Catalyst</t>
+  </si>
+  <si>
+    <t>Atziris Disfavour</t>
+  </si>
+  <si>
+    <t>Triumvirate Authority</t>
+  </si>
+  <si>
+    <t>Doryanis Invitation</t>
+  </si>
+  <si>
+    <t>Mortal Grief</t>
+  </si>
+  <si>
+    <t>Mortal Ignorance</t>
+  </si>
+  <si>
+    <t>Mortal Hope</t>
+  </si>
+  <si>
+    <t>Mortal Rage</t>
+  </si>
+  <si>
+    <t>Sacrificial Garb</t>
+  </si>
+  <si>
+    <t>uber elder</t>
+  </si>
+  <si>
+    <t>Mark of the Shaper</t>
+  </si>
+  <si>
+    <t>Mark of the Elder</t>
+  </si>
+  <si>
+    <t>Indigon</t>
+  </si>
+  <si>
+    <t>Call of the Void</t>
+  </si>
+  <si>
+    <t>Voidfletcher</t>
+  </si>
+  <si>
+    <t>Disintegrator</t>
+  </si>
+  <si>
+    <t>Voidforge</t>
+  </si>
+  <si>
+    <t>The Eternity Shroud</t>
+  </si>
+  <si>
+    <t>Soul Ascension</t>
+  </si>
+  <si>
+    <t>Decaying Reliquary Key</t>
+  </si>
+  <si>
+    <t>uber atziri</t>
+  </si>
+  <si>
+    <t>Atziris Acuity</t>
+  </si>
+  <si>
+    <t>Atziris Reflection</t>
+  </si>
+  <si>
+    <t>Atziris Rule</t>
+  </si>
+  <si>
+    <t>The Vertex</t>
+  </si>
+  <si>
+    <t>Atziris Splendour</t>
+  </si>
+  <si>
+    <t>Pledge of Hands</t>
+  </si>
+  <si>
+    <t>Victorious Fate</t>
+  </si>
+  <si>
+    <t>maven</t>
+  </si>
+  <si>
+    <t>Legacy of Fury</t>
+  </si>
+  <si>
+    <t>Viridis Veil</t>
+  </si>
+  <si>
+    <t>Arns Anguish</t>
+  </si>
+  <si>
+    <t>Gravens Secret</t>
+  </si>
+  <si>
+    <t>Olesyas Delight</t>
+  </si>
+  <si>
+    <t>Impossible Escape</t>
+  </si>
+  <si>
+    <t>Doppelgänger Guise</t>
+  </si>
+  <si>
+    <t>Shiny Reliquary Key</t>
+  </si>
+  <si>
+    <t>Elevated Sextant</t>
+  </si>
+  <si>
+    <t>Orb of Conflict</t>
+  </si>
+  <si>
+    <t>sirus</t>
+  </si>
+  <si>
+    <t>Crown of the Inward Eye</t>
+  </si>
+  <si>
+    <t>Hands of the High Templar</t>
+  </si>
+  <si>
+    <t>Thread of Hope (small - very large)</t>
+  </si>
+  <si>
+    <t>The Burden of Truth</t>
+  </si>
+  <si>
+    <t>The Saviour</t>
+  </si>
+  <si>
+    <t>Thread of Hope (massive)</t>
+  </si>
+  <si>
+    <t>Oubliette Reliquary Key</t>
+  </si>
+  <si>
+    <t>Awakeners Orb</t>
+  </si>
+  <si>
+    <t>Awakened Support Gems</t>
+  </si>
+  <si>
+    <t>Awakened Exceptional Support Gems</t>
+  </si>
+  <si>
+    <t>Blasphemers Grasp</t>
+  </si>
+  <si>
+    <t>Solstice Vigil</t>
+  </si>
+  <si>
+    <t>Echoes of Creation</t>
   </si>
 </sst>
 </file>
@@ -435,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1D2404-1E0A-46B7-8772-FEDC11F371AC}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,6 +687,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -457,7 +700,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -465,16 +708,16 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2">
         <v>50</v>
       </c>
       <c r="D2">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -482,16 +725,16 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3">
         <v>50</v>
       </c>
       <c r="D3">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="E3">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -499,75 +742,117 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>50</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>25</v>
       </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6">
         <v>12</v>
       </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>94</v>
       </c>
       <c r="C8">
         <v>5</v>
       </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>95</v>
       </c>
       <c r="C9">
         <v>5</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <v>4</v>
       </c>
     </row>
@@ -576,7 +861,16 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>69</v>
+      </c>
+      <c r="D11">
+        <v>69</v>
+      </c>
+      <c r="E11">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -584,13 +878,1376 @@
         <v>0</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
+      <c r="D12">
+        <v>69</v>
+      </c>
       <c r="E12">
         <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>50</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14">
+        <v>50</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15">
+        <v>25</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>25</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>10</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21">
+        <v>5</v>
+      </c>
+      <c r="D21">
+        <v>69</v>
+      </c>
+      <c r="E21">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>25</v>
+      </c>
+      <c r="D22">
+        <v>10</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>69</v>
+      </c>
+      <c r="E23">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>69</v>
+      </c>
+      <c r="D24">
+        <v>69</v>
+      </c>
+      <c r="E24">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>69</v>
+      </c>
+      <c r="E25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26">
+        <v>69</v>
+      </c>
+      <c r="D26">
+        <v>69</v>
+      </c>
+      <c r="E26">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27">
+        <v>69</v>
+      </c>
+      <c r="D27">
+        <v>69</v>
+      </c>
+      <c r="E27">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>69</v>
+      </c>
+      <c r="E28">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29">
+        <v>69</v>
+      </c>
+      <c r="D29">
+        <v>69</v>
+      </c>
+      <c r="E29">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30">
+        <v>69</v>
+      </c>
+      <c r="D30">
+        <v>69</v>
+      </c>
+      <c r="E30">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31">
+        <v>69</v>
+      </c>
+      <c r="D31">
+        <v>69</v>
+      </c>
+      <c r="E31">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32">
+        <v>69</v>
+      </c>
+      <c r="D32">
+        <v>69</v>
+      </c>
+      <c r="E32">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33">
+        <v>69</v>
+      </c>
+      <c r="D33">
+        <v>69</v>
+      </c>
+      <c r="E33">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34">
+        <v>69</v>
+      </c>
+      <c r="D34">
+        <v>69</v>
+      </c>
+      <c r="E34">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35">
+        <v>69</v>
+      </c>
+      <c r="D35">
+        <v>69</v>
+      </c>
+      <c r="E35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C36">
+        <v>69</v>
+      </c>
+      <c r="D36">
+        <v>69</v>
+      </c>
+      <c r="E36">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>40</v>
+      </c>
+      <c r="B37" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37">
+        <v>69</v>
+      </c>
+      <c r="D37">
+        <v>69</v>
+      </c>
+      <c r="E37">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38">
+        <v>69</v>
+      </c>
+      <c r="D38">
+        <v>69</v>
+      </c>
+      <c r="E38">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39">
+        <v>69</v>
+      </c>
+      <c r="D39">
+        <v>69</v>
+      </c>
+      <c r="E39">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40">
+        <v>69</v>
+      </c>
+      <c r="D40">
+        <v>69</v>
+      </c>
+      <c r="E40">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41">
+        <v>69</v>
+      </c>
+      <c r="D41">
+        <v>69</v>
+      </c>
+      <c r="E41">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42">
+        <v>69</v>
+      </c>
+      <c r="D42">
+        <v>69</v>
+      </c>
+      <c r="E42">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43">
+        <v>69</v>
+      </c>
+      <c r="D43">
+        <v>69</v>
+      </c>
+      <c r="E43">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>69</v>
+      </c>
+      <c r="D44">
+        <v>69</v>
+      </c>
+      <c r="E44">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45">
+        <v>69</v>
+      </c>
+      <c r="D45">
+        <v>69</v>
+      </c>
+      <c r="E45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46">
+        <v>69</v>
+      </c>
+      <c r="D46">
+        <v>69</v>
+      </c>
+      <c r="E46">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>40</v>
+      </c>
+      <c r="B47" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47">
+        <v>69</v>
+      </c>
+      <c r="D47">
+        <v>69</v>
+      </c>
+      <c r="E47">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48">
+        <v>69</v>
+      </c>
+      <c r="D48">
+        <v>69</v>
+      </c>
+      <c r="E48">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>52</v>
+      </c>
+      <c r="B49" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49">
+        <v>69</v>
+      </c>
+      <c r="D49">
+        <v>69</v>
+      </c>
+      <c r="E49">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50">
+        <v>69</v>
+      </c>
+      <c r="D50">
+        <v>69</v>
+      </c>
+      <c r="E50">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51">
+        <v>69</v>
+      </c>
+      <c r="D51">
+        <v>69</v>
+      </c>
+      <c r="E51">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>57</v>
+      </c>
+      <c r="C52">
+        <v>69</v>
+      </c>
+      <c r="D52">
+        <v>69</v>
+      </c>
+      <c r="E52">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53">
+        <v>69</v>
+      </c>
+      <c r="D53">
+        <v>69</v>
+      </c>
+      <c r="E53">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>59</v>
+      </c>
+      <c r="C54">
+        <v>69</v>
+      </c>
+      <c r="D54">
+        <v>69</v>
+      </c>
+      <c r="E54">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" t="s">
+        <v>60</v>
+      </c>
+      <c r="C55">
+        <v>69</v>
+      </c>
+      <c r="D55">
+        <v>69</v>
+      </c>
+      <c r="E55">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>52</v>
+      </c>
+      <c r="B56" t="s">
+        <v>21</v>
+      </c>
+      <c r="C56">
+        <v>69</v>
+      </c>
+      <c r="D56">
+        <v>69</v>
+      </c>
+      <c r="E56">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>52</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57">
+        <v>69</v>
+      </c>
+      <c r="D57">
+        <v>69</v>
+      </c>
+      <c r="E57">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>52</v>
+      </c>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58">
+        <v>69</v>
+      </c>
+      <c r="D58">
+        <v>69</v>
+      </c>
+      <c r="E58">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B59" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59">
+        <v>69</v>
+      </c>
+      <c r="D59">
+        <v>69</v>
+      </c>
+      <c r="E59">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>52</v>
+      </c>
+      <c r="B60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>69</v>
+      </c>
+      <c r="D60">
+        <v>69</v>
+      </c>
+      <c r="E60">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" t="s">
+        <v>12</v>
+      </c>
+      <c r="C61">
+        <v>69</v>
+      </c>
+      <c r="D61">
+        <v>69</v>
+      </c>
+      <c r="E61">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
+        <v>64</v>
+      </c>
+      <c r="C62">
+        <v>69</v>
+      </c>
+      <c r="D62">
+        <v>69</v>
+      </c>
+      <c r="E62">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>65</v>
+      </c>
+      <c r="C63">
+        <v>69</v>
+      </c>
+      <c r="D63">
+        <v>69</v>
+      </c>
+      <c r="E63">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64">
+        <v>69</v>
+      </c>
+      <c r="D64">
+        <v>69</v>
+      </c>
+      <c r="E64">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65">
+        <v>69</v>
+      </c>
+      <c r="D65">
+        <v>69</v>
+      </c>
+      <c r="E65">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>63</v>
+      </c>
+      <c r="B66" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66">
+        <v>69</v>
+      </c>
+      <c r="D66">
+        <v>69</v>
+      </c>
+      <c r="E66">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67" t="s">
+        <v>68</v>
+      </c>
+      <c r="C67">
+        <v>69</v>
+      </c>
+      <c r="D67">
+        <v>69</v>
+      </c>
+      <c r="E67">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>63</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68">
+        <v>69</v>
+      </c>
+      <c r="D68">
+        <v>69</v>
+      </c>
+      <c r="E68">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>63</v>
+      </c>
+      <c r="B69" t="s">
+        <v>51</v>
+      </c>
+      <c r="C69">
+        <v>69</v>
+      </c>
+      <c r="D69">
+        <v>69</v>
+      </c>
+      <c r="E69">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>63</v>
+      </c>
+      <c r="B70" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70">
+        <v>69</v>
+      </c>
+      <c r="D70">
+        <v>69</v>
+      </c>
+      <c r="E70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>72</v>
+      </c>
+      <c r="C71">
+        <v>69</v>
+      </c>
+      <c r="D71">
+        <v>69</v>
+      </c>
+      <c r="E71">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>73</v>
+      </c>
+      <c r="C72">
+        <v>69</v>
+      </c>
+      <c r="D72">
+        <v>69</v>
+      </c>
+      <c r="E72">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73">
+        <v>69</v>
+      </c>
+      <c r="D73">
+        <v>69</v>
+      </c>
+      <c r="E73">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74" t="s">
+        <v>75</v>
+      </c>
+      <c r="C74">
+        <v>69</v>
+      </c>
+      <c r="D74">
+        <v>69</v>
+      </c>
+      <c r="E74">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>71</v>
+      </c>
+      <c r="B75" t="s">
+        <v>76</v>
+      </c>
+      <c r="C75">
+        <v>69</v>
+      </c>
+      <c r="D75">
+        <v>69</v>
+      </c>
+      <c r="E75">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76">
+        <v>69</v>
+      </c>
+      <c r="D76">
+        <v>69</v>
+      </c>
+      <c r="E76">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>71</v>
+      </c>
+      <c r="B77" t="s">
+        <v>78</v>
+      </c>
+      <c r="C77">
+        <v>69</v>
+      </c>
+      <c r="D77">
+        <v>69</v>
+      </c>
+      <c r="E77">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>71</v>
+      </c>
+      <c r="B78" t="s">
+        <v>92</v>
+      </c>
+      <c r="C78">
+        <v>69</v>
+      </c>
+      <c r="D78">
+        <v>69</v>
+      </c>
+      <c r="E78">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>71</v>
+      </c>
+      <c r="B79" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79">
+        <v>69</v>
+      </c>
+      <c r="D79">
+        <v>69</v>
+      </c>
+      <c r="E79">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>71</v>
+      </c>
+      <c r="B80" t="s">
+        <v>80</v>
+      </c>
+      <c r="C80">
+        <v>69</v>
+      </c>
+      <c r="D80">
+        <v>69</v>
+      </c>
+      <c r="E80">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>71</v>
+      </c>
+      <c r="B81" t="s">
+        <v>81</v>
+      </c>
+      <c r="C81">
+        <v>69</v>
+      </c>
+      <c r="D81">
+        <v>69</v>
+      </c>
+      <c r="E81">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>71</v>
+      </c>
+      <c r="B82" t="s">
+        <v>91</v>
+      </c>
+      <c r="C82">
+        <v>69</v>
+      </c>
+      <c r="D82">
+        <v>69</v>
+      </c>
+      <c r="E82">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>83</v>
+      </c>
+      <c r="C83">
+        <v>69</v>
+      </c>
+      <c r="D83">
+        <v>69</v>
+      </c>
+      <c r="E83">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>84</v>
+      </c>
+      <c r="C84">
+        <v>69</v>
+      </c>
+      <c r="D84">
+        <v>69</v>
+      </c>
+      <c r="E84">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>82</v>
+      </c>
+      <c r="B85" t="s">
+        <v>85</v>
+      </c>
+      <c r="C85">
+        <v>69</v>
+      </c>
+      <c r="D85">
+        <v>69</v>
+      </c>
+      <c r="E85">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86" t="s">
+        <v>86</v>
+      </c>
+      <c r="C86">
+        <v>69</v>
+      </c>
+      <c r="D86">
+        <v>69</v>
+      </c>
+      <c r="E86">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" t="s">
+        <v>87</v>
+      </c>
+      <c r="C87">
+        <v>69</v>
+      </c>
+      <c r="D87">
+        <v>69</v>
+      </c>
+      <c r="E87">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>82</v>
+      </c>
+      <c r="B88" t="s">
+        <v>88</v>
+      </c>
+      <c r="C88">
+        <v>69</v>
+      </c>
+      <c r="D88">
+        <v>69</v>
+      </c>
+      <c r="E88">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89" t="s">
+        <v>89</v>
+      </c>
+      <c r="C89">
+        <v>69</v>
+      </c>
+      <c r="D89">
+        <v>69</v>
+      </c>
+      <c r="E89">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90" t="s">
+        <v>91</v>
+      </c>
+      <c r="C90">
+        <v>69</v>
+      </c>
+      <c r="D90">
+        <v>69</v>
+      </c>
+      <c r="E90">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>82</v>
+      </c>
+      <c r="B91" t="s">
+        <v>12</v>
+      </c>
+      <c r="C91">
+        <v>69</v>
+      </c>
+      <c r="D91">
+        <v>69</v>
+      </c>
+      <c r="E91">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>82</v>
+      </c>
+      <c r="B92" t="s">
+        <v>90</v>
+      </c>
+      <c r="C92">
+        <v>69</v>
+      </c>
+      <c r="D92">
+        <v>69</v>
+      </c>
+      <c r="E92">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated odds with poe.how
</commit_message>
<xml_diff>
--- a/Odds.xlsx
+++ b/Odds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aqua\Documents\GitHub\PoeProfit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E4151E-D7C0-4578-91CF-7F1CAFA55FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA5470DB-D908-484F-937A-B838CD249FDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1575" yWindow="3420" windowWidth="31560" windowHeight="15435" xr2:uid="{577F8554-80CD-4CC0-9DB5-09CB9B2401F0}"/>
   </bookViews>
@@ -680,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1D2404-1E0A-46B7-8772-FEDC11F371AC}">
   <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="C90" sqref="C90"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C92" sqref="C92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -748,7 +748,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>51.5</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -765,7 +765,7 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -782,7 +782,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -799,7 +799,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -833,13 +833,13 @@
         <v>95</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>10.47</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -884,13 +884,13 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1071,7 +1071,7 @@
         <v>25</v>
       </c>
       <c r="C23">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -1088,7 +1088,7 @@
         <v>26</v>
       </c>
       <c r="C24">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -1105,7 +1105,7 @@
         <v>28</v>
       </c>
       <c r="C25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -1139,13 +1139,13 @@
         <v>29</v>
       </c>
       <c r="C27">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D27">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1179,7 +1179,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1190,7 +1190,7 @@
         <v>33</v>
       </c>
       <c r="C30">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -1207,7 +1207,7 @@
         <v>34</v>
       </c>
       <c r="C31">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -1224,7 +1224,7 @@
         <v>35</v>
       </c>
       <c r="C32">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -1258,13 +1258,13 @@
         <v>37</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D34">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,7 +1298,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
         <v>41</v>
       </c>
       <c r="C37">
-        <v>62</v>
+        <v>67.97</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -1326,7 +1326,7 @@
         <v>42</v>
       </c>
       <c r="C38">
-        <v>15</v>
+        <v>12.2</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -1343,7 +1343,7 @@
         <v>43</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>4.58</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -1394,7 +1394,7 @@
         <v>46</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>15.25</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -1411,7 +1411,7 @@
         <v>47</v>
       </c>
       <c r="C43">
-        <v>16</v>
+        <v>15.47</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -1428,7 +1428,7 @@
         <v>48</v>
       </c>
       <c r="C44">
-        <v>8</v>
+        <v>10.68</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -1445,7 +1445,7 @@
         <v>49</v>
       </c>
       <c r="C45">
-        <v>5</v>
+        <v>5.23</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -1462,7 +1462,7 @@
         <v>50</v>
       </c>
       <c r="C46">
-        <v>12</v>
+        <v>10.02</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -1479,7 +1479,7 @@
         <v>51</v>
       </c>
       <c r="C47">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -1530,7 +1530,7 @@
         <v>55</v>
       </c>
       <c r="C50">
-        <v>12</v>
+        <v>16.88</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -1547,13 +1547,13 @@
         <v>56</v>
       </c>
       <c r="C51">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1564,7 +1564,7 @@
         <v>57</v>
       </c>
       <c r="C52">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -1581,7 +1581,7 @@
         <v>58</v>
       </c>
       <c r="C53">
-        <v>6</v>
+        <v>7.5</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -1598,13 +1598,13 @@
         <v>59</v>
       </c>
       <c r="C54">
+        <v>3</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
         <v>2</v>
-      </c>
-      <c r="D54">
-        <v>0</v>
-      </c>
-      <c r="E54">
-        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1734,7 +1734,7 @@
         <v>64</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>3.48</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -1785,7 +1785,7 @@
         <v>67</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>46.52</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -1819,7 +1819,7 @@
         <v>68</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>37.81</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -1887,7 +1887,7 @@
         <v>72</v>
       </c>
       <c r="C71">
-        <v>32</v>
+        <v>26.15</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -1904,7 +1904,7 @@
         <v>73</v>
       </c>
       <c r="C72">
-        <v>20</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -1921,7 +1921,7 @@
         <v>74</v>
       </c>
       <c r="C73">
-        <v>12</v>
+        <v>24.62</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -1938,7 +1938,7 @@
         <v>75</v>
       </c>
       <c r="C74">
-        <v>12</v>
+        <v>16.920000000000002</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -1955,7 +1955,7 @@
         <v>76</v>
       </c>
       <c r="C75">
-        <v>12</v>
+        <v>12.31</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -1989,7 +1989,7 @@
         <v>78</v>
       </c>
       <c r="C77">
-        <v>2</v>
+        <v>2.44</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -2023,7 +2023,7 @@
         <v>79</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>2.36</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -2040,13 +2040,14 @@
         <v>80</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>49.23</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80">
-        <v>100</v>
+        <f>100-C80</f>
+        <v>50.77</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2109,7 +2110,7 @@
         <v>84</v>
       </c>
       <c r="C84">
-        <v>25</v>
+        <v>34.72</v>
       </c>
       <c r="D84">
         <v>0</v>

</xml_diff>